<commit_message>
Modificaciones finales a la clase 03/09/24 terminadas
</commit_message>
<xml_diff>
--- a/Ejercicios en clase/Clase 5 03 09 24/clase 04 09 24 excel.xlsx
+++ b/Ejercicios en clase/Clase 5 03 09 24/clase 04 09 24 excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/931d574390e6cf0b/Documentos/ITS Semestre 11/LAB VISION COMPUTACIONAL/Filtros/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/931d574390e6cf0b/Documentos/ITS Semestre 11/VISION COMPUTACIONAL/Ejercicios en clase/Clase 5 03 09 24/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{1D418FDF-7F7F-4FDE-B241-7C08393A2B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0927738-5381-4E0A-B29C-8EEF5B4E851C}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{1D418FDF-7F7F-4FDE-B241-7C08393A2B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74172D35-09E6-48F7-AD81-2AD1CF478FF8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{FA83C4D0-4986-430C-B812-4A8B614A9A83}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FA83C4D0-4986-430C-B812-4A8B614A9A83}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -185,6 +185,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -212,10 +213,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -538,21 +535,21 @@
   <dimension ref="B1:J38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="3">
         <v>232</v>
       </c>
@@ -572,7 +569,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="3">
         <v>215</v>
       </c>
@@ -595,7 +592,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="3">
         <v>230</v>
       </c>
@@ -618,7 +615,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="3">
         <v>215</v>
       </c>
@@ -638,7 +635,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="3">
         <v>224</v>
       </c>
@@ -658,12 +655,12 @@
         <v>215</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H7">
         <v>215</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <f>AVERAGE(B2:F6)</f>
         <v>213.28</v>
@@ -675,30 +672,30 @@
         <v>217</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H9">
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="15" t="s">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
       <c r="H10">
         <v>219</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4">
-        <f t="shared" ref="B11:F15" si="0">(ABS(B2-$B$8)*100/$B$8)</f>
+        <f>(ABS(B2-$B$8)*100/$B$8)</f>
         <v>8.7771942985746438</v>
       </c>
       <c r="C11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B11:F15" si="0">(ABS(C2-$B$8)*100/$B$8)</f>
         <v>5.0262565641410353</v>
       </c>
       <c r="D11" s="8">
@@ -717,7 +714,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4">
         <f t="shared" si="0"/>
         <v>0.80645161290322531</v>
@@ -742,7 +739,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="4">
         <f t="shared" si="0"/>
         <v>7.8394598649662415</v>
@@ -767,7 +764,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="4">
         <f t="shared" si="0"/>
         <v>0.80645161290322531</v>
@@ -793,7 +790,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <f t="shared" si="0"/>
         <v>5.0262565641410353</v>
@@ -819,25 +816,25 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="H16">
         <v>226</v>
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B17" s="15" t="s">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
       <c r="H17">
         <v>228</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3">
         <v>232</v>
       </c>
@@ -845,7 +842,7 @@
         <v>224</v>
       </c>
       <c r="D18" s="9">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="E18" s="3">
         <v>232</v>
@@ -858,7 +855,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3">
         <v>215</v>
       </c>
@@ -872,14 +869,14 @@
         <v>230</v>
       </c>
       <c r="F19" s="9">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="H19">
         <v>230</v>
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3">
         <v>230</v>
       </c>
@@ -900,12 +897,12 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3">
         <v>215</v>
       </c>
       <c r="C21" s="9">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="D21" s="3">
         <v>228</v>
@@ -920,7 +917,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3">
         <v>224</v>
       </c>
@@ -941,16 +938,16 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>232</v>
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <f>AVERAGE(B18:F22)</f>
-        <v>226.92</v>
+        <v>226.2</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>1</v>
@@ -960,157 +957,158 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H25">
         <v>233</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B26" s="15" t="s">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
       <c r="H26">
         <v>234</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="4">
         <f t="shared" ref="B27:F31" si="1">(ABS(B18-$B$24)*100/$B$24)</f>
-        <v>2.2386744227040425</v>
+        <v>2.5641025641025692</v>
       </c>
       <c r="C27" s="4">
         <f t="shared" si="1"/>
-        <v>1.2867971091133386</v>
+        <v>0.97259062776303662</v>
       </c>
       <c r="D27" s="4">
         <f t="shared" si="1"/>
-        <v>2.2386744227040425</v>
+        <v>8.8417329796635122E-2</v>
       </c>
       <c r="E27" s="4">
         <f t="shared" si="1"/>
-        <v>2.2386744227040425</v>
+        <v>2.5641025641025692</v>
       </c>
       <c r="F27" s="4">
         <f t="shared" si="1"/>
-        <v>2.6793583641812151</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+        <v>3.0061892130857699</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="4">
         <f t="shared" si="1"/>
-        <v>5.2529525824078913</v>
+        <v>4.9513704686118434</v>
       </c>
       <c r="C28" s="4">
         <f t="shared" si="1"/>
-        <v>1.7979904812268697</v>
+        <v>2.1220159151193685</v>
       </c>
       <c r="D28" s="4">
         <f t="shared" si="1"/>
-        <v>3.1200423056583877</v>
+        <v>3.4482758620689706</v>
       </c>
       <c r="E28" s="4">
         <f t="shared" si="1"/>
-        <v>1.3573065397496971</v>
+        <v>1.6799292661361678</v>
       </c>
       <c r="F28" s="4">
         <f t="shared" si="1"/>
-        <v>2.2386744227040425</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+        <v>8.8417329796635122E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="4">
         <f t="shared" si="1"/>
-        <v>1.3573065397496971</v>
+        <v>1.6799292661361678</v>
       </c>
       <c r="C29" s="4">
         <f t="shared" si="1"/>
-        <v>3.9309007579763739</v>
+        <v>3.6251105216622408</v>
       </c>
       <c r="D29" s="4">
         <f t="shared" si="1"/>
-        <v>0.40542922615899329</v>
+        <v>8.8417329796635122E-2</v>
       </c>
       <c r="E29" s="4">
         <f t="shared" si="1"/>
-        <v>3.4902168164992013</v>
+        <v>3.1830238726790401</v>
       </c>
       <c r="F29" s="4">
         <f t="shared" si="1"/>
-        <v>0.40542922615899329</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+        <v>8.8417329796635122E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="4">
         <f t="shared" si="1"/>
-        <v>5.2529525824078913</v>
+        <v>4.9513704686118434</v>
       </c>
       <c r="C30" s="4">
         <f t="shared" si="1"/>
-        <v>2.2386744227040425</v>
+        <v>8.8417329796635122E-2</v>
       </c>
       <c r="D30" s="4">
         <f t="shared" si="1"/>
-        <v>0.47593865679535191</v>
+        <v>0.79575596816976635</v>
       </c>
       <c r="E30" s="4">
         <f t="shared" si="1"/>
-        <v>1.3573065397496971</v>
+        <v>1.6799292661361678</v>
       </c>
       <c r="F30" s="4">
         <f t="shared" si="1"/>
-        <v>2.2386744227040425</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+        <v>2.5641025641025692</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="4">
         <f t="shared" si="1"/>
-        <v>1.2867971091133386</v>
+        <v>0.97259062776303662</v>
       </c>
       <c r="C31" s="4">
         <f t="shared" si="1"/>
-        <v>2.6088489335448561</v>
+        <v>2.2988505747126387</v>
       </c>
       <c r="D31" s="4">
         <f t="shared" si="1"/>
-        <v>3.1200423056583877</v>
+        <v>3.4482758620689706</v>
       </c>
       <c r="E31" s="4">
         <f t="shared" si="1"/>
-        <v>0.40542922615899329</v>
+        <v>8.8417329796635122E-2</v>
       </c>
       <c r="F31" s="4">
         <f t="shared" si="1"/>
-        <v>4.371584699453547</v>
+        <v>4.067197170645442</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G32" s="5">
         <f>SUM(B27:F31)</f>
-        <v>57.394676537986982</v>
-      </c>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="16" t="s">
+        <v>51.105216622457988</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F34" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="G34" s="16"/>
-    </row>
-    <row r="35" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="17"/>
+    </row>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F35" s="11">
         <v>226</v>
       </c>
       <c r="G35" s="3">
         <v>51.11</v>
       </c>
-    </row>
-    <row r="36" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="H35" s="15"/>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F36" s="14">
         <v>226</v>
       </c>
@@ -1118,7 +1116,7 @@
         <v>51.11</v>
       </c>
     </row>
-    <row r="37" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F37" s="14">
         <v>230</v>
       </c>
@@ -1126,7 +1124,7 @@
         <v>55.13</v>
       </c>
     </row>
-    <row r="38" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:8" x14ac:dyDescent="0.25">
       <c r="F38" s="14">
         <v>232</v>
       </c>

</xml_diff>